<commit_message>
8/4 thermo computer changes
</commit_message>
<xml_diff>
--- a/QAQCS.xlsx
+++ b/QAQCS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1425" yWindow="1425" windowWidth="21600" windowHeight="11385" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="QAQCs" sheetId="1" state="visible" r:id="rId1"/>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4225" uniqueCount="4225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4228" uniqueCount="4228">
   <si>
     <t>HRE.p1Std.112020</t>
   </si>
@@ -12688,6 +12688,15 @@
   </si>
   <si>
     <t xml:space="preserve">CLU120_06_250505</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLU_05_250804</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLU_01_250804</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLUTEST_02_250804</t>
   </si>
 </sst>
 </file>
@@ -13508,7 +13517,9 @@
       <c r="D36" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E36"/>
+      <c r="E36" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
@@ -13521,7 +13532,9 @@
       <c r="D37" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E37"/>
+      <c r="E37" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
@@ -14521,7 +14534,9 @@
       <c r="D113" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E113"/>
+      <c r="E113" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="s">
@@ -15775,7 +15790,9 @@
       <c r="D209" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E209"/>
+      <c r="E209" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="s">
@@ -17159,7 +17176,9 @@
       <c r="D315" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E315"/>
+      <c r="E315" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="s">
@@ -18378,7 +18397,9 @@
       <c r="D408" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E408"/>
+      <c r="E408" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="409">
       <c r="A409" s="1" t="s">
@@ -19541,7 +19562,9 @@
       <c r="D497" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E497"/>
+      <c r="E497" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="498">
       <c r="A498" s="1" t="s">
@@ -20795,7 +20818,9 @@
       <c r="D593" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E593"/>
+      <c r="E593" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="594">
       <c r="A594" s="1" t="s">
@@ -22049,7 +22074,9 @@
       <c r="D689" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E689"/>
+      <c r="E689" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="690">
       <c r="A690" s="1" t="s">
@@ -23303,7 +23330,9 @@
       <c r="D785" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E785"/>
+      <c r="E785" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="786">
       <c r="A786" s="1" t="s">
@@ -24791,7 +24820,9 @@
       <c r="D899" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E899"/>
+      <c r="E899" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="900">
       <c r="A900" s="1" t="s">
@@ -24804,7 +24835,9 @@
       <c r="D900" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E900"/>
+      <c r="E900" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="901">
       <c r="A901" s="1" t="s">
@@ -37746,7 +37779,9 @@
       <c r="D1892" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1892"/>
+      <c r="E1892" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="1893">
       <c r="A1893" t="s">
@@ -37759,7 +37794,9 @@
       <c r="D1893" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1893"/>
+      <c r="E1893" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="1894">
       <c r="A1894" t="s">
@@ -37772,7 +37809,9 @@
       <c r="D1894" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1894"/>
+      <c r="E1894" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="1895">
       <c r="A1895" t="s">
@@ -37785,7 +37824,9 @@
       <c r="D1895" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1895"/>
+      <c r="E1895" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="1896">
       <c r="A1896" t="s">
@@ -37798,7 +37839,9 @@
       <c r="D1896" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1896"/>
+      <c r="E1896" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="1897">
       <c r="A1897" t="s">
@@ -37811,7 +37854,9 @@
       <c r="D1897" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1897"/>
+      <c r="E1897" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="1898">
       <c r="A1898" t="s">
@@ -37824,7 +37869,9 @@
       <c r="D1898" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1898"/>
+      <c r="E1898" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="1899">
       <c r="A1899" t="s">
@@ -37837,7 +37884,9 @@
       <c r="D1899" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1899"/>
+      <c r="E1899" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="1900">
       <c r="A1900" t="s">
@@ -38188,7 +38237,9 @@
       <c r="D1926" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1926"/>
+      <c r="E1926" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="1927">
       <c r="A1927" t="s">
@@ -38201,7 +38252,9 @@
       <c r="D1927" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1927"/>
+      <c r="E1927" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="1928">
       <c r="A1928" t="s">
@@ -38546,7 +38599,9 @@
       <c r="D1952" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1952"/>
+      <c r="E1952" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="1953">
       <c r="A1953" t="s">
@@ -38559,7 +38614,9 @@
       <c r="D1953" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1953"/>
+      <c r="E1953" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="1954">
       <c r="A1954" t="s">
@@ -38572,7 +38629,9 @@
       <c r="D1954" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1954"/>
+      <c r="E1954" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="1955">
       <c r="A1955" t="s">
@@ -38585,7 +38644,9 @@
       <c r="D1955" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1955"/>
+      <c r="E1955" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="1956">
       <c r="A1956" t="s">
@@ -38598,7 +38659,9 @@
       <c r="D1956" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1956"/>
+      <c r="E1956" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="1957">
       <c r="A1957" t="s">
@@ -38611,7 +38674,9 @@
       <c r="D1957" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1957"/>
+      <c r="E1957" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="1958">
       <c r="A1958" t="s">
@@ -38624,7 +38689,9 @@
       <c r="D1958" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1958"/>
+      <c r="E1958" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="1959">
       <c r="A1959" t="s">
@@ -38637,7 +38704,9 @@
       <c r="D1959" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1959"/>
+      <c r="E1959" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="1960">
       <c r="A1960" t="s">
@@ -39014,7 +39083,9 @@
       <c r="D1988" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1988"/>
+      <c r="E1988" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="1989">
       <c r="A1989" t="s">
@@ -39027,7 +39098,9 @@
       <c r="D1989" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1989"/>
+      <c r="E1989" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="1990">
       <c r="A1990" t="s">
@@ -39255,7 +39328,9 @@
       <c r="D2005" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E2005"/>
+      <c r="E2005" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="2006">
       <c r="A2006" t="s">
@@ -39359,7 +39434,9 @@
       <c r="D2013" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E2013"/>
+      <c r="E2013" t="s">
+        <v>4227</v>
+      </c>
     </row>
     <row r="2014">
       <c r="A2014" t="s">

</xml_diff>

<commit_message>
8/7 changes lab computer not much
</commit_message>
<xml_diff>
--- a/QAQCS.xlsx
+++ b/QAQCS.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4230" uniqueCount="4230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4231" uniqueCount="4231">
   <si>
     <t>HRE.p1Std.112020</t>
   </si>
@@ -12703,6 +12703,9 @@
   </si>
   <si>
     <t xml:space="preserve">CLUTEST_07_250805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLUTEST_03_250807</t>
   </si>
 </sst>
 </file>
@@ -13557,7 +13560,9 @@
       <c r="D38" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E38"/>
+      <c r="E38" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
@@ -13570,7 +13575,9 @@
       <c r="D39" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E39"/>
+      <c r="E39" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
@@ -14561,7 +14568,9 @@
       <c r="D114" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E114"/>
+      <c r="E114" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="s">
@@ -15819,7 +15828,9 @@
       <c r="D210" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E210"/>
+      <c r="E210" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="s">
@@ -17209,7 +17220,9 @@
       <c r="D316" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E316"/>
+      <c r="E316" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="s">
@@ -18378,7 +18391,9 @@
       <c r="D405" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E405"/>
+      <c r="E405" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="406">
       <c r="A406" s="1" t="s">
@@ -19599,7 +19614,9 @@
       <c r="D498" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E498"/>
+      <c r="E498" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="499">
       <c r="A499" s="1" t="s">
@@ -20857,7 +20874,9 @@
       <c r="D594" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E594"/>
+      <c r="E594" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="595">
       <c r="A595" s="1" t="s">
@@ -22115,7 +22134,9 @@
       <c r="D690" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E690"/>
+      <c r="E690" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="691">
       <c r="A691" s="1" t="s">
@@ -23373,7 +23394,9 @@
       <c r="D786" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E786"/>
+      <c r="E786" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="787">
       <c r="A787" s="1" t="s">
@@ -24882,7 +24905,9 @@
       <c r="D901" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E901"/>
+      <c r="E901" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="902">
       <c r="A902" s="1" t="s">
@@ -24895,7 +24920,9 @@
       <c r="D902" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E902"/>
+      <c r="E902" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="903">
       <c r="A903" s="1" t="s">
@@ -33596,7 +33623,9 @@
       <c r="D1565" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1565"/>
+      <c r="E1565" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="1566">
       <c r="A1566" s="1" t="s">
@@ -37979,7 +38008,9 @@
       <c r="D1900" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1900"/>
+      <c r="E1900" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="1901">
       <c r="A1901" t="s">
@@ -37992,7 +38023,9 @@
       <c r="D1901" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1901"/>
+      <c r="E1901" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="1902">
       <c r="A1902" t="s">
@@ -38005,7 +38038,9 @@
       <c r="D1902" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1902"/>
+      <c r="E1902" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="1903">
       <c r="A1903" t="s">
@@ -38018,7 +38053,9 @@
       <c r="D1903" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1903"/>
+      <c r="E1903" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="1904">
       <c r="A1904" t="s">
@@ -38031,7 +38068,9 @@
       <c r="D1904" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1904"/>
+      <c r="E1904" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="1905">
       <c r="A1905" t="s">
@@ -38044,7 +38083,9 @@
       <c r="D1905" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1905"/>
+      <c r="E1905" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="1906">
       <c r="A1906" t="s">
@@ -38057,7 +38098,9 @@
       <c r="D1906" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1906"/>
+      <c r="E1906" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="1907">
       <c r="A1907" t="s">
@@ -38070,7 +38113,9 @@
       <c r="D1907" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1907"/>
+      <c r="E1907" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="1908">
       <c r="A1908" t="s">
@@ -38347,7 +38392,9 @@
       <c r="D1928" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1928"/>
+      <c r="E1928" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="1929">
       <c r="A1929" t="s">
@@ -38360,7 +38407,9 @@
       <c r="D1929" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1929"/>
+      <c r="E1929" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="1930">
       <c r="A1930" t="s">
@@ -38799,7 +38848,9 @@
       <c r="D1960" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1960"/>
+      <c r="E1960" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="1961">
       <c r="A1961" t="s">
@@ -38812,7 +38863,9 @@
       <c r="D1961" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1961"/>
+      <c r="E1961" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="1962">
       <c r="A1962" t="s">
@@ -38825,7 +38878,9 @@
       <c r="D1962" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1962"/>
+      <c r="E1962" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="1963">
       <c r="A1963" t="s">
@@ -38838,7 +38893,9 @@
       <c r="D1963" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1963"/>
+      <c r="E1963" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="1964">
       <c r="A1964" t="s">
@@ -38851,7 +38908,9 @@
       <c r="D1964" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1964"/>
+      <c r="E1964" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="1965">
       <c r="A1965" t="s">
@@ -38864,7 +38923,9 @@
       <c r="D1965" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1965"/>
+      <c r="E1965" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="1966">
       <c r="A1966" t="s">
@@ -38877,7 +38938,9 @@
       <c r="D1966" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1966"/>
+      <c r="E1966" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="1967">
       <c r="A1967" t="s">
@@ -38890,7 +38953,9 @@
       <c r="D1967" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1967"/>
+      <c r="E1967" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="1968">
       <c r="A1968" t="s">
@@ -39137,7 +39202,9 @@
       <c r="D1986" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1986"/>
+      <c r="E1986" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="1987">
       <c r="A1987" t="s">
@@ -39150,7 +39217,9 @@
       <c r="D1987" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1987"/>
+      <c r="E1987" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="1988">
       <c r="A1988" t="s">
@@ -39423,7 +39492,9 @@
       <c r="D2006" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E2006"/>
+      <c r="E2006" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="2007">
       <c r="A2007" t="s">
@@ -39529,7 +39600,9 @@
       <c r="D2014" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E2014"/>
+      <c r="E2014" t="s">
+        <v>4230</v>
+      </c>
     </row>
     <row r="2015">
       <c r="A2015" t="s">

</xml_diff>

<commit_message>
8/8 lab lots of changes
</commit_message>
<xml_diff>
--- a/QAQCS.xlsx
+++ b/QAQCS.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4231" uniqueCount="4231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4232" uniqueCount="4232">
   <si>
     <t>HRE.p1Std.112020</t>
   </si>
@@ -12706,6 +12706,9 @@
   </si>
   <si>
     <t xml:space="preserve">CLUTEST_03_250807</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLUTEST_04_250808</t>
   </si>
 </sst>
 </file>
@@ -13561,7 +13564,7 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="39">
@@ -13576,7 +13579,7 @@
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="40">
@@ -13616,7 +13619,9 @@
       <c r="D42" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E42"/>
+      <c r="E42" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
@@ -13629,7 +13634,9 @@
       <c r="D43" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E43"/>
+      <c r="E43" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
@@ -14569,7 +14576,7 @@
         <v>1</v>
       </c>
       <c r="E114" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="115">
@@ -14596,7 +14603,9 @@
       <c r="D116" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E116"/>
+      <c r="E116" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="s">
@@ -15829,7 +15838,7 @@
         <v>1</v>
       </c>
       <c r="E210" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="211">
@@ -15856,7 +15865,9 @@
       <c r="D212" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E212"/>
+      <c r="E212" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="s">
@@ -17221,7 +17232,7 @@
         <v>1</v>
       </c>
       <c r="E316" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="317">
@@ -17248,7 +17259,9 @@
       <c r="D318" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E318"/>
+      <c r="E318" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="s">
@@ -18392,7 +18405,7 @@
         <v>1</v>
       </c>
       <c r="E405" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="406">
@@ -18419,7 +18432,9 @@
       <c r="D407" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E407"/>
+      <c r="E407" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="408">
       <c r="A408" s="1" t="s">
@@ -19615,7 +19630,7 @@
         <v>1</v>
       </c>
       <c r="E498" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="499">
@@ -19642,7 +19657,9 @@
       <c r="D500" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E500"/>
+      <c r="E500" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="501">
       <c r="A501" s="1" t="s">
@@ -20875,7 +20892,7 @@
         <v>1</v>
       </c>
       <c r="E594" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="595">
@@ -20902,7 +20919,9 @@
       <c r="D596" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E596"/>
+      <c r="E596" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="597">
       <c r="A597" s="1" t="s">
@@ -22135,7 +22154,7 @@
         <v>1</v>
       </c>
       <c r="E690" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="691">
@@ -22162,7 +22181,9 @@
       <c r="D692" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E692"/>
+      <c r="E692" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="693">
       <c r="A693" s="1" t="s">
@@ -23395,7 +23416,7 @@
         <v>1</v>
       </c>
       <c r="E786" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="787">
@@ -23422,7 +23443,9 @@
       <c r="D788" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E788"/>
+      <c r="E788" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="789">
       <c r="A789" s="1" t="s">
@@ -24906,7 +24929,7 @@
         <v>1</v>
       </c>
       <c r="E901" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="902">
@@ -24921,7 +24944,7 @@
         <v>1</v>
       </c>
       <c r="E902" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="903">
@@ -24961,7 +24984,9 @@
       <c r="D905" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E905"/>
+      <c r="E905" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="906">
       <c r="A906" s="1" t="s">
@@ -24974,7 +24999,9 @@
       <c r="D906" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E906"/>
+      <c r="E906" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="907">
       <c r="A907" s="1" t="s">
@@ -33624,7 +33651,7 @@
         <v>1</v>
       </c>
       <c r="E1565" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="1566">
@@ -38009,7 +38036,7 @@
         <v>1</v>
       </c>
       <c r="E1900" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="1901">
@@ -38024,7 +38051,7 @@
         <v>1</v>
       </c>
       <c r="E1901" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="1902">
@@ -38039,7 +38066,7 @@
         <v>1</v>
       </c>
       <c r="E1902" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="1903">
@@ -38054,7 +38081,7 @@
         <v>1</v>
       </c>
       <c r="E1903" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="1904">
@@ -38069,7 +38096,7 @@
         <v>1</v>
       </c>
       <c r="E1904" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="1905">
@@ -38084,7 +38111,7 @@
         <v>1</v>
       </c>
       <c r="E1905" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="1906">
@@ -38099,7 +38126,7 @@
         <v>1</v>
       </c>
       <c r="E1906" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="1907">
@@ -38114,7 +38141,7 @@
         <v>1</v>
       </c>
       <c r="E1907" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="1908">
@@ -38232,7 +38259,9 @@
       <c r="D1916" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1916"/>
+      <c r="E1916" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="1917">
       <c r="A1917" t="s">
@@ -38245,7 +38274,9 @@
       <c r="D1917" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1917"/>
+      <c r="E1917" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="1918">
       <c r="A1918" t="s">
@@ -38258,7 +38289,9 @@
       <c r="D1918" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1918"/>
+      <c r="E1918" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="1919">
       <c r="A1919" t="s">
@@ -38271,7 +38304,9 @@
       <c r="D1919" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1919"/>
+      <c r="E1919" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="1920">
       <c r="A1920" t="s">
@@ -38284,7 +38319,9 @@
       <c r="D1920" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1920"/>
+      <c r="E1920" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="1921">
       <c r="A1921" t="s">
@@ -38297,7 +38334,9 @@
       <c r="D1921" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1921"/>
+      <c r="E1921" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="1922">
       <c r="A1922" t="s">
@@ -38310,7 +38349,9 @@
       <c r="D1922" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1922"/>
+      <c r="E1922" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="1923">
       <c r="A1923" t="s">
@@ -38323,7 +38364,9 @@
       <c r="D1923" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1923"/>
+      <c r="E1923" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="1924">
       <c r="A1924" t="s">
@@ -38393,7 +38436,7 @@
         <v>1</v>
       </c>
       <c r="E1928" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="1929">
@@ -38408,7 +38451,7 @@
         <v>1</v>
       </c>
       <c r="E1929" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="1930">
@@ -38448,7 +38491,9 @@
       <c r="D1932" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1932"/>
+      <c r="E1932" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="1933">
       <c r="A1933" t="s">
@@ -38461,7 +38506,9 @@
       <c r="D1933" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1933"/>
+      <c r="E1933" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="1934">
       <c r="A1934" t="s">
@@ -38849,7 +38896,7 @@
         <v>1</v>
       </c>
       <c r="E1960" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="1961">
@@ -38864,7 +38911,7 @@
         <v>1</v>
       </c>
       <c r="E1961" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="1962">
@@ -38879,7 +38926,7 @@
         <v>1</v>
       </c>
       <c r="E1962" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="1963">
@@ -38894,7 +38941,7 @@
         <v>1</v>
       </c>
       <c r="E1963" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="1964">
@@ -38909,7 +38956,7 @@
         <v>1</v>
       </c>
       <c r="E1964" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="1965">
@@ -38924,7 +38971,7 @@
         <v>1</v>
       </c>
       <c r="E1965" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="1966">
@@ -38939,7 +38986,7 @@
         <v>1</v>
       </c>
       <c r="E1966" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="1967">
@@ -38954,7 +39001,7 @@
         <v>1</v>
       </c>
       <c r="E1967" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="1968">
@@ -39072,7 +39119,9 @@
       <c r="D1976" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1976"/>
+      <c r="E1976" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="1977">
       <c r="A1977" t="s">
@@ -39085,7 +39134,9 @@
       <c r="D1977" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1977"/>
+      <c r="E1977" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="1978">
       <c r="A1978" t="s">
@@ -39098,7 +39149,9 @@
       <c r="D1978" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1978"/>
+      <c r="E1978" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="1979">
       <c r="A1979" t="s">
@@ -39111,7 +39164,9 @@
       <c r="D1979" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1979"/>
+      <c r="E1979" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="1980">
       <c r="A1980" t="s">
@@ -39124,7 +39179,9 @@
       <c r="D1980" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1980"/>
+      <c r="E1980" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="1981">
       <c r="A1981" t="s">
@@ -39137,7 +39194,9 @@
       <c r="D1981" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1981"/>
+      <c r="E1981" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="1982">
       <c r="A1982" t="s">
@@ -39150,7 +39209,9 @@
       <c r="D1982" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1982"/>
+      <c r="E1982" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="1983">
       <c r="A1983" t="s">
@@ -39163,7 +39224,9 @@
       <c r="D1983" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1983"/>
+      <c r="E1983" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="1984">
       <c r="A1984" t="s">
@@ -39203,7 +39266,7 @@
         <v>1</v>
       </c>
       <c r="E1986" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="1987">
@@ -39218,7 +39281,7 @@
         <v>1</v>
       </c>
       <c r="E1987" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="1988">
@@ -39378,7 +39441,9 @@
       <c r="D1998" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1998"/>
+      <c r="E1998" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="1999">
       <c r="A1999" t="s">
@@ -39391,7 +39456,9 @@
       <c r="D1999" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1999"/>
+      <c r="E1999" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="2000">
       <c r="A2000" t="s">
@@ -39493,7 +39560,7 @@
         <v>1</v>
       </c>
       <c r="E2006" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="2007">
@@ -39520,7 +39587,9 @@
       <c r="D2008" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E2008"/>
+      <c r="E2008" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="2009">
       <c r="A2009" t="s">
@@ -39601,7 +39670,7 @@
         <v>1</v>
       </c>
       <c r="E2014" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="2015">
@@ -39628,7 +39697,9 @@
       <c r="D2016" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E2016"/>
+      <c r="E2016" t="s">
+        <v>4231</v>
+      </c>
     </row>
     <row r="2017">
       <c r="A2017" t="s">

</xml_diff>